<commit_message>
adding t-tests for classifiers
</commit_message>
<xml_diff>
--- a/docs/Classifcation Reports/DecisionTreeClassifier()_1.xlsx
+++ b/docs/Classifcation Reports/DecisionTreeClassifier()_1.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7996575342465754</v>
+        <v>0.7828668363019508</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8017167381974248</v>
+        <v>0.7984429065743944</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8006858122588942</v>
+        <v>0.7905781584582441</v>
       </c>
       <c r="E2" t="n">
-        <v>1165</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.838258164852255</v>
+        <v>0.8717948717948718</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8343653250773994</v>
+        <v>0.785824345146379</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8363072148952676</v>
+        <v>0.826580226904376</v>
       </c>
       <c r="E3" t="n">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7394957983193278</v>
+        <v>0.7551282051282051</v>
       </c>
       <c r="C4" t="n">
-        <v>0.796895213454075</v>
+        <v>0.7474619289340102</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7671232876712328</v>
+        <v>0.7512755102040817</v>
       </c>
       <c r="E4" t="n">
-        <v>773</v>
+        <v>788</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6182432432432432</v>
+        <v>0.4974747474747475</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5140449438202247</v>
+        <v>0.5677233429394812</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5613496932515338</v>
+        <v>0.5302826379542396</v>
       </c>
       <c r="E5" t="n">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7727891156462585</v>
+        <v>0.7547619047619047</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7727891156462585</v>
+        <v>0.7547619047619047</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7727891156462585</v>
+        <v>0.7547619047619047</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7727891156462585</v>
+        <v>0.7547619047619047</v>
       </c>
     </row>
     <row r="7">
@@ -557,13 +557,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7489136851653504</v>
+        <v>0.7268161651749437</v>
       </c>
       <c r="C7" t="n">
-        <v>0.736755555137281</v>
+        <v>0.7248631308985662</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7413665020192322</v>
+        <v>0.7246791333802354</v>
       </c>
       <c r="E7" t="n">
         <v>2940</v>
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7703539621045075</v>
+        <v>0.761378808698874</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7727891156462585</v>
+        <v>0.7547619047619047</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7707075592759739</v>
+        <v>0.7572694203570095</v>
       </c>
       <c r="E8" t="n">
         <v>2940</v>

</xml_diff>